<commit_message>
CU checkear, Avance CRNG
</commit_message>
<xml_diff>
--- a/Planificación/Casos de Uso.xlsx
+++ b/Planificación/Casos de Uso.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\intec\OneDrive\Escritorio\intecTroquian\Planificación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B1AF64-9B70-49F3-A30A-25730E1CBB10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2D70D8-BFC8-4DF9-B2BF-448D8242EA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CU-001" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="174">
   <si>
     <t>Versión</t>
   </si>
@@ -495,6 +495,99 @@
   </si>
   <si>
     <t>Los usuarios con permisos de administración pueden utilizar el Módulo D sin restricciones.</t>
+  </si>
+  <si>
+    <t>Visualización de Estadísticas Clave sobre Lotes de Trabajo</t>
+  </si>
+  <si>
+    <t>CU-011</t>
+  </si>
+  <si>
+    <t>RF-29</t>
+  </si>
+  <si>
+    <t>Este caso de uso describe cómo un usuario accede al sistema para visualizar estadísticas clave relacionadas con los lotes de trabajo, específicamente el número de lotes creados dentro de un rango de tiempo definido.</t>
+  </si>
+  <si>
+    <t>El usuario debe estar autenticado y tener permisos para acceder al módulo de estadísticas.
+Deben existir registros de lotes de trabajo en el sistema.</t>
+  </si>
+  <si>
+    <t>El usuario accede al sistema con sus credenciales.</t>
+  </si>
+  <si>
+    <t>El usuario Navega al módulo de estadísticas.</t>
+  </si>
+  <si>
+    <t>El sistema Muestra las diferentes estadísticas disponibles para su visualización.</t>
+  </si>
+  <si>
+    <t>El usuario Selecciona la opción "Número de lotes de trabajo creados" y define un rango de fechas</t>
+  </si>
+  <si>
+    <t>El sistema Consulta la base de datos para obtener los lotes de trabajo creados dentro del período seleccionado.</t>
+  </si>
+  <si>
+    <t>El sistema Muestra el número total de lotes de trabajo creados durante el período especificado.</t>
+  </si>
+  <si>
+    <t>El usuario visualiza el número de lotes de trabajo creados durante el período de tiempo especificado.</t>
+  </si>
+  <si>
+    <t>Se recomienda que el sistema muestre gráficos o tablas que faciliten la interpretación de los datos de manera visual.</t>
+  </si>
+  <si>
+    <t>RF-30</t>
+  </si>
+  <si>
+    <t>CU-012</t>
+  </si>
+  <si>
+    <t>Búsqueda de Lotes de Trabajo con Múltiples Filtros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Este caso de uso describe cómo los usuarios pueden buscar lotes de trabajo en el sistema utilizando diferentes filtros como la fecha de creación, el responsable del lote, el estado del lote y otros criterios.
+</t>
+  </si>
+  <si>
+    <t>El usuario debe estar autenticado y tener permisos para acceder al módulo de búsqueda de lotes de trabajo.
+Deben existir registros de lotes de trabajo en el sistema.</t>
+  </si>
+  <si>
+    <t>Administrador, Digitador VISA, Digitador INTECIL</t>
+  </si>
+  <si>
+    <t>El usuario visualiza una lista de lotes de trabajo que coinciden con los filtros aplicados.</t>
+  </si>
+  <si>
+    <t>El tiempo de respuesta del sistema debe ser óptimo, incluso cuando se apliquen múltiples filtros.</t>
+  </si>
+  <si>
+    <t>El usuario selecciona los filtros deseados</t>
+  </si>
+  <si>
+    <t>El sistema muestra la interfaz de búsqueda con opciones para aplicar filtros (fecha de creación, responsable, estado del lote, etc.).</t>
+  </si>
+  <si>
+    <t>El usuario navega al módulo de búsqueda de lotes de trabajo.</t>
+  </si>
+  <si>
+    <t>El sistema verifica las credenciales y los permisos del usuario.</t>
+  </si>
+  <si>
+    <t>El usuario hace clic en el botón "Buscar"</t>
+  </si>
+  <si>
+    <t>El sistema consulta la base de datos utilizando los filtros seleccionados y muestra una lista de lotes de trabajo que coinciden con los criterios.</t>
+  </si>
+  <si>
+    <t>El usuario visualiza los resultados de la búsqueda y puede hacer clic en un lote de trabajo específico para ver más detalles.</t>
+  </si>
+  <si>
+    <t>Si no se encuentran lotes de trabajo que coincidan con los filtros seleccionados el sistema muestra un mensaje indicando que no se encontraron resultados para los criterios de búsqueda.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si no existen lotes de trabajo creados en el período seleccionado muestra un mensaje indicando que no se encontraron lotes de trabajo </t>
   </si>
 </sst>
 </file>
@@ -1340,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477D27A8-6762-4728-B78B-D2BFAC47D9CD}">
-  <dimension ref="B3:D21"/>
+  <dimension ref="B3:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1355,10 +1448,10 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -1376,7 +1469,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="D5" s="16"/>
     </row>
@@ -1385,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="D6" s="13"/>
     </row>
@@ -1394,7 +1487,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D7" s="12"/>
     </row>
@@ -1424,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -1433,7 +1526,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -1442,7 +1535,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
@@ -1451,7 +1544,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -1460,64 +1553,60 @@
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C15" s="7">
+        <v>6</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="D20" s="16"/>
-    </row>
-    <row r="21" spans="2:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
+      <c r="C18" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="D18" s="16"/>
+    </row>
+    <row r="19" spans="2:4" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
@@ -1534,22 +1623,22 @@
   <dimension ref="B3:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D21"/>
+      <selection activeCell="C20" sqref="C20:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21.5546875" customWidth="1"/>
     <col min="3" max="3" width="6.5546875" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="108.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>133</v>
+        <v>159</v>
       </c>
       <c r="D3" s="14"/>
     </row>
@@ -1567,7 +1656,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="D5" s="16"/>
     </row>
@@ -1576,16 +1665,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="2:4" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D7" s="12"/>
     </row>
@@ -1594,7 +1683,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>63</v>
+        <v>162</v>
       </c>
       <c r="D8" s="16"/>
     </row>
@@ -1615,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>123</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
@@ -1624,7 +1713,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.3">
@@ -1633,7 +1722,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
@@ -1642,7 +1731,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.3">
@@ -1651,23 +1740,29 @@
         <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="16" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="17" spans="2:4" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="3"/>
+      <c r="D17" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
@@ -1686,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1694,7 +1789,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="D20" s="16"/>
     </row>
@@ -1702,7 +1797,9 @@
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>164</v>
+      </c>
       <c r="D21" s="12"/>
     </row>
   </sheetData>
@@ -1882,7 +1979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A32A5BF-2D70-4BC7-A352-7C53E7059BA8}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>